<commit_message>
Correct mfr part no of single row header
</commit_message>
<xml_diff>
--- a/notes/1802-Mini-Compact-Flash-BOM.xlsx
+++ b/notes/1802-Mini-Compact-Flash-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C83EE3B-0E52-4AC8-AA8D-A192F23F6AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E002417-EEA9-40FF-AB71-C8111FF13554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18120" yWindow="-120" windowWidth="18240" windowHeight="28590" xr2:uid="{41E1A1E5-C1FC-4043-9E65-8CBBFB1D39B7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
   <si>
     <t>Jumper shunts 0.1"</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Socket 20 pin 0.1" long tail (*B) (*C)</t>
+  </si>
+  <si>
+    <t>PREC040SAAN-RC</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
   <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1455,7 +1458,7 @@
         <v>36</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>12</v>

</xml_diff>